<commit_message>
Added 2000 milisecond delay after clicking send button
</commit_message>
<xml_diff>
--- a/LinkedIn_Connect/LinkedIn_Links.xlsx
+++ b/LinkedIn_Connect/LinkedIn_Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nainksha\RPA\uipath_automation\LinkedIn_Connect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C9771D-4E5F-4C70-8462-F741011CF683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3181ABCD-498F-4390-8272-DD26C0C55403}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,48 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>LinkedIn_Links</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/sreebalaji/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/bala-bharadvaj-0400871/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/rajni-singh-50a1825/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/ashwani-bhargava-40975990/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/mohemmed-ansari-45572427/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/amitabh1kumar/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/dr-akhil-prasad-9a6a5b4/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/ravi-8b78baa9/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/surendra-ahuja-103a7369/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/michael-koch-4b02635/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/faizi-mohsini-b10a5027/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/salil-gupte-0a7bb86/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/ritu-sandhu-sharma-b3664817/</t>
   </si>
   <si>
     <t>https://www.linkedin.com/in/happy-mohanty-7b52115/</t>
@@ -678,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A130"/>
+  <dimension ref="A1:A117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="66.109375" defaultRowHeight="18.75" customHeight="1"/>
@@ -697,11 +658,11 @@
     </row>
     <row r="2" spans="1:1" ht="18.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -751,67 +712,67 @@
       </c>
     </row>
     <row r="13" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -821,7 +782,7 @@
       </c>
     </row>
     <row r="27" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -831,7 +792,7 @@
       </c>
     </row>
     <row r="29" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -846,12 +807,12 @@
       </c>
     </row>
     <row r="32" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -886,7 +847,7 @@
       </c>
     </row>
     <row r="40" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -911,7 +872,7 @@
       </c>
     </row>
     <row r="45" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -946,12 +907,12 @@
       </c>
     </row>
     <row r="52" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -966,7 +927,7 @@
       </c>
     </row>
     <row r="56" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -991,7 +952,7 @@
       </c>
     </row>
     <row r="61" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1011,7 +972,7 @@
       </c>
     </row>
     <row r="65" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="5" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1026,12 +987,12 @@
       </c>
     </row>
     <row r="68" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="5" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1056,7 +1017,7 @@
       </c>
     </row>
     <row r="74" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="5" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1086,12 +1047,12 @@
       </c>
     </row>
     <row r="80" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="5" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1101,69 +1062,43 @@
       </c>
     </row>
     <row r="83" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A83" s="5" t="s">
-        <v>81</v>
-      </c>
+      <c r="A83" s="6"/>
     </row>
     <row r="84" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A84" s="5" t="s">
-        <v>82</v>
-      </c>
+      <c r="A84" s="6"/>
     </row>
     <row r="85" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A85" s="5" t="s">
-        <v>83</v>
-      </c>
+      <c r="A85" s="6"/>
     </row>
     <row r="86" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A86" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="A86" s="6"/>
     </row>
     <row r="87" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A87" s="5" t="s">
-        <v>85</v>
-      </c>
+      <c r="A87" s="6"/>
     </row>
     <row r="88" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A88" s="5" t="s">
-        <v>86</v>
-      </c>
+      <c r="A88" s="6"/>
     </row>
     <row r="89" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A89" s="5" t="s">
-        <v>87</v>
-      </c>
+      <c r="A89" s="6"/>
     </row>
     <row r="90" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A90" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="A90" s="6"/>
     </row>
     <row r="91" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A91" s="5" t="s">
-        <v>89</v>
-      </c>
+      <c r="A91" s="6"/>
     </row>
     <row r="92" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A92" s="5" t="s">
-        <v>90</v>
-      </c>
+      <c r="A92" s="6"/>
     </row>
     <row r="93" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A93" s="3" t="s">
-        <v>91</v>
-      </c>
+      <c r="A93" s="6"/>
     </row>
     <row r="94" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A94" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="A94" s="6"/>
     </row>
     <row r="95" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A95" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="A95" s="6"/>
     </row>
     <row r="96" spans="1:1" ht="18.75" customHeight="1">
       <c r="A96" s="6"/>
@@ -1231,143 +1166,91 @@
     <row r="117" spans="1:1" ht="18.75" customHeight="1">
       <c r="A117" s="6"/>
     </row>
-    <row r="118" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A118" s="6"/>
-    </row>
-    <row r="119" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A119" s="6"/>
-    </row>
-    <row r="120" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A120" s="6"/>
-    </row>
-    <row r="121" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A121" s="6"/>
-    </row>
-    <row r="122" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A122" s="6"/>
-    </row>
-    <row r="123" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A123" s="6"/>
-    </row>
-    <row r="124" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A124" s="6"/>
-    </row>
-    <row r="125" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A125" s="6"/>
-    </row>
-    <row r="126" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A126" s="6"/>
-    </row>
-    <row r="127" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A127" s="6"/>
-    </row>
-    <row r="128" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A128" s="6"/>
-    </row>
-    <row r="129" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A129" s="6"/>
-    </row>
-    <row r="130" spans="1:1" ht="18.75" customHeight="1">
-      <c r="A130" s="6"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{A6D4819F-1B16-4109-B817-6E7F53CAC052}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{A0B1F1A6-04D8-47D8-AA40-ECFA50A7D93F}"/>
-    <hyperlink ref="A5" r:id="rId3" xr:uid="{B9625046-6693-47FD-A8E0-FD7A87ECEDFD}"/>
-    <hyperlink ref="A6" r:id="rId4" xr:uid="{95D55870-FAB7-413C-8800-4315468D6AE2}"/>
-    <hyperlink ref="A7" r:id="rId5" xr:uid="{4AADED4D-10C2-418D-8CF7-EBE8C7335E62}"/>
-    <hyperlink ref="A8" r:id="rId6" xr:uid="{CDCCEB06-1FC1-40F2-9C4A-00AF0E99AD6A}"/>
-    <hyperlink ref="A9" r:id="rId7" xr:uid="{99E6F72C-B3A5-45FB-BF7F-32E3CB04CF02}"/>
-    <hyperlink ref="A10" r:id="rId8" xr:uid="{0C4F27B3-0F37-4BF9-B8AC-E5029E9EF40B}"/>
-    <hyperlink ref="A11" r:id="rId9" xr:uid="{3F9FCC95-54F9-44D3-9567-180452A57A6F}"/>
-    <hyperlink ref="A12" r:id="rId10" xr:uid="{ECD6ABBB-E3C0-4710-AE75-2895190D3615}"/>
-    <hyperlink ref="A13" r:id="rId11" xr:uid="{A98444C2-5186-49A9-A9B9-4803D62AE784}"/>
-    <hyperlink ref="A14" r:id="rId12" xr:uid="{B38C5485-2B3D-47A7-95EB-96342EC050F5}"/>
-    <hyperlink ref="A15" r:id="rId13" xr:uid="{A78BA3C2-5E5C-4AA8-8967-DDCDB992450F}"/>
-    <hyperlink ref="A16" r:id="rId14" xr:uid="{2ED6477F-0688-4D70-9365-BC7C4E376E82}"/>
-    <hyperlink ref="A17" r:id="rId15" xr:uid="{4E965D07-00A3-4210-A3BD-0610EC11A2A9}"/>
-    <hyperlink ref="A18" r:id="rId16" xr:uid="{AD3154FD-4E59-4F6A-AF7A-0BD20636047C}"/>
-    <hyperlink ref="A19" r:id="rId17" xr:uid="{C83CACB8-67C6-4F79-9BDF-1044B79921D5}"/>
-    <hyperlink ref="A20" r:id="rId18" xr:uid="{D43AE3EF-E3DA-41C8-AFC4-E5349EC8B5C5}"/>
-    <hyperlink ref="A21" r:id="rId19" xr:uid="{4BB1437E-9B8A-40C0-B9C6-4EFE0F984E0C}"/>
-    <hyperlink ref="A22" r:id="rId20" xr:uid="{D6BE7778-74BB-4963-ABA9-ADD3BC183450}"/>
-    <hyperlink ref="A23" r:id="rId21" xr:uid="{5B12592E-5270-4F77-A890-6AC575B216BE}"/>
-    <hyperlink ref="A24" r:id="rId22" xr:uid="{5EDFA56F-BCE8-4595-8022-78A9EC20F81C}"/>
-    <hyperlink ref="A25" r:id="rId23" xr:uid="{8F9FB0A6-1066-4016-99F3-F077C1A61B72}"/>
-    <hyperlink ref="A26" r:id="rId24" xr:uid="{ECCE968F-15BA-40FE-84E4-AA690F0243C3}"/>
-    <hyperlink ref="A27" r:id="rId25" xr:uid="{A7D770FF-8719-4845-B12A-369B078A57AF}"/>
-    <hyperlink ref="A28" r:id="rId26" xr:uid="{B8E2B792-248D-4E06-A44A-37FB0751C926}"/>
-    <hyperlink ref="A29" r:id="rId27" xr:uid="{33FE71A4-3055-4512-9648-835FF72B73A0}"/>
-    <hyperlink ref="A30" r:id="rId28" xr:uid="{CB5A3C4C-13D9-4B24-B195-210ED4FBE9DD}"/>
-    <hyperlink ref="A31" r:id="rId29" xr:uid="{3AC92931-509C-42A2-B8B3-B8E9825C6152}"/>
-    <hyperlink ref="A32" r:id="rId30" xr:uid="{D481EA02-ABB2-477A-B879-64A8985E8B70}"/>
-    <hyperlink ref="A33" r:id="rId31" xr:uid="{2BA13EA5-BEF4-4BD6-9DC5-1712C7F0D6AD}"/>
-    <hyperlink ref="A34" r:id="rId32" xr:uid="{A1CC8ACA-57E9-426C-AD55-3D98FB8F4A3C}"/>
-    <hyperlink ref="A35" r:id="rId33" xr:uid="{1D7C8697-430A-4635-98F7-6C07C74C047A}"/>
-    <hyperlink ref="A36" r:id="rId34" xr:uid="{15CFAEC5-E79E-4A81-BA48-14FC39B0936A}"/>
-    <hyperlink ref="A37" r:id="rId35" xr:uid="{442ADA00-59A2-4E20-A46E-763B9C9B3C61}"/>
-    <hyperlink ref="A38" r:id="rId36" xr:uid="{780A9EF4-0D73-4CA9-9D8C-044E7EA952B6}"/>
-    <hyperlink ref="A39" r:id="rId37" xr:uid="{BCE3420B-4685-430C-BF85-F07AF758B484}"/>
-    <hyperlink ref="A40" r:id="rId38" xr:uid="{57291359-7B98-4B4C-8536-8EB7441B14A0}"/>
-    <hyperlink ref="A41" r:id="rId39" xr:uid="{9D67495D-89E1-4FDD-99B2-CC69FB31AF9E}"/>
-    <hyperlink ref="A42" r:id="rId40" xr:uid="{A226A6D0-E373-442F-AB5F-E0B292A02A8A}"/>
-    <hyperlink ref="A43" r:id="rId41" xr:uid="{41817B1D-9404-48C4-B75D-F3D8B9E0AD1D}"/>
-    <hyperlink ref="A44" r:id="rId42" xr:uid="{EB71C670-C4CE-4398-BDE7-77300FD16A0D}"/>
-    <hyperlink ref="A45" r:id="rId43" xr:uid="{D4C6CE7D-0BC7-48E8-ADDB-23A197EACE2E}"/>
-    <hyperlink ref="A46" r:id="rId44" xr:uid="{44B8E59E-0510-4D97-870C-C3C231B24295}"/>
-    <hyperlink ref="A47" r:id="rId45" xr:uid="{506D721A-9121-4CE4-BDE2-6298F5AC0A80}"/>
-    <hyperlink ref="A48" r:id="rId46" xr:uid="{3705B74A-ADF1-4299-9614-AA3121DAA70E}"/>
-    <hyperlink ref="A49" r:id="rId47" xr:uid="{BEAD36FD-1FCD-4EB6-B097-565D30DEEE06}"/>
-    <hyperlink ref="A50" r:id="rId48" xr:uid="{426CE7E4-A72D-4063-BD29-E92B5F2639B4}"/>
-    <hyperlink ref="A51" r:id="rId49" xr:uid="{D42F1856-FFB3-4C86-AB39-3C7E6526AAD3}"/>
-    <hyperlink ref="A52" r:id="rId50" xr:uid="{74522C41-48D1-4AF6-A507-54A73C6E8B60}"/>
-    <hyperlink ref="A53" r:id="rId51" xr:uid="{FD599B93-4AD7-40AE-8E60-8B8214FB0CA9}"/>
-    <hyperlink ref="A54" r:id="rId52" xr:uid="{BC65FEAA-46EB-44A4-941A-1A1ACE394565}"/>
-    <hyperlink ref="A55" r:id="rId53" xr:uid="{BDE6EB0D-79F9-44D0-8443-3D7CB8C14462}"/>
-    <hyperlink ref="A56" r:id="rId54" xr:uid="{CAC9B4DB-E9A6-4438-B269-D09E1BC8548F}"/>
-    <hyperlink ref="A57" r:id="rId55" xr:uid="{DDFA5ABF-AE8F-49FA-A3B7-21A4DE9ED7F4}"/>
-    <hyperlink ref="A58" r:id="rId56" xr:uid="{BBBA4BAB-6646-4FEC-9A4F-4C76BDB17FC1}"/>
-    <hyperlink ref="A59" r:id="rId57" xr:uid="{451C84BC-237E-4282-87A3-46FBC0F6D86D}"/>
-    <hyperlink ref="A60" r:id="rId58" xr:uid="{2F75B136-F1C2-4C12-B624-31ECE87D8A47}"/>
-    <hyperlink ref="A61" r:id="rId59" xr:uid="{CDA32D37-0E6E-4DB6-8996-1391D6B823AF}"/>
-    <hyperlink ref="A62" r:id="rId60" xr:uid="{A8E3D0EC-CE2B-49A6-825B-9F3A98A84902}"/>
-    <hyperlink ref="A63" r:id="rId61" xr:uid="{91BE7A6B-AB8E-4217-9051-99D643CFB8B9}"/>
-    <hyperlink ref="A64" r:id="rId62" xr:uid="{66C6D3CB-1799-4DC3-BA4B-9F2067186376}"/>
-    <hyperlink ref="A65" r:id="rId63" xr:uid="{967DFBB0-D1D8-4869-8CAD-65D686C4C122}"/>
-    <hyperlink ref="A66" r:id="rId64" xr:uid="{BE4394CD-4739-4374-8B48-AE4A22F6EBA8}"/>
-    <hyperlink ref="A67" r:id="rId65" xr:uid="{70FD45C9-805A-4576-B677-EFC5E8BCBEB0}"/>
-    <hyperlink ref="A68" r:id="rId66" xr:uid="{E0A82E61-FA34-4A2F-88C1-1D90A6B43CA9}"/>
-    <hyperlink ref="A69" r:id="rId67" xr:uid="{16E2E0B9-865F-47A9-A2DF-60DC29575AA3}"/>
-    <hyperlink ref="A70" r:id="rId68" xr:uid="{27711C84-8F4E-4452-8FCF-A565AFA74D4B}"/>
-    <hyperlink ref="A71" r:id="rId69" xr:uid="{062B4421-F4D8-4DD2-90E7-81C270D8DB40}"/>
-    <hyperlink ref="A72" r:id="rId70" xr:uid="{5515994B-B7C3-45F0-ACAA-B4F27271573A}"/>
-    <hyperlink ref="A73" r:id="rId71" xr:uid="{36EEE2B9-2129-4E3E-86EB-D45FF5CD0362}"/>
-    <hyperlink ref="A74" r:id="rId72" xr:uid="{8DC9732E-558E-4A1A-B05E-23B317DB8187}"/>
-    <hyperlink ref="A75" r:id="rId73" xr:uid="{DE39333C-BED3-46A7-A6C3-E74790E4838A}"/>
-    <hyperlink ref="A76" r:id="rId74" xr:uid="{EF628698-ACEB-4818-8438-8AE9DBE4E126}"/>
-    <hyperlink ref="A77" r:id="rId75" xr:uid="{A5E3A352-1658-4385-AA61-C5534A3A9587}"/>
-    <hyperlink ref="A78" r:id="rId76" xr:uid="{4AE2E7BA-0779-480A-9E10-833E8BEE6176}"/>
-    <hyperlink ref="A79" r:id="rId77" xr:uid="{B3B16C79-E44A-4AE2-B5C9-1EFD3F70716F}"/>
-    <hyperlink ref="A80" r:id="rId78" xr:uid="{03DA74CC-C5B3-4A14-A92E-53593A6ED634}"/>
-    <hyperlink ref="A81" r:id="rId79" xr:uid="{292707FA-9363-4D5D-85B0-DE717207FB57}"/>
-    <hyperlink ref="A82" r:id="rId80" xr:uid="{762A6932-B76D-4288-AAA5-AD7B947816CD}"/>
-    <hyperlink ref="A83" r:id="rId81" xr:uid="{A7A1FE0D-E7F4-4EAE-9CF9-CAFF7CD89E4B}"/>
-    <hyperlink ref="A84" r:id="rId82" xr:uid="{390820E8-74CF-4356-A8B3-BCE3EF7CD95D}"/>
-    <hyperlink ref="A85" r:id="rId83" xr:uid="{8327DA18-AD6F-40E6-ACEE-D696E19D77BE}"/>
-    <hyperlink ref="A86" r:id="rId84" xr:uid="{FB7730C5-19E4-46CB-B430-BA67FB7A8BF6}"/>
-    <hyperlink ref="A87" r:id="rId85" xr:uid="{5C886BAE-5C7E-43DC-9F0F-6D2E48017393}"/>
-    <hyperlink ref="A88" r:id="rId86" xr:uid="{DD617D6F-76F1-4B6B-A91A-BD297C6E5B2F}"/>
-    <hyperlink ref="A89" r:id="rId87" xr:uid="{149414E2-2F48-42D0-A11E-07B59A54E26C}"/>
-    <hyperlink ref="A90" r:id="rId88" xr:uid="{93D0BD43-2609-492E-AD0E-DE9EAC41013B}"/>
-    <hyperlink ref="A91" r:id="rId89" xr:uid="{6AAE379F-5B4B-4BAC-A622-2C0B9A6D27C8}"/>
-    <hyperlink ref="A92" r:id="rId90" xr:uid="{8E61AF1B-D8B7-4E8E-A65E-A37974FCCEDE}"/>
-    <hyperlink ref="A93" r:id="rId91" xr:uid="{0D32D76B-A1CC-4E22-BFB0-1657FDF52326}"/>
-    <hyperlink ref="A94" r:id="rId92" xr:uid="{88E2535D-E2EA-4BB4-B2A8-61F8D7CC7094}"/>
-    <hyperlink ref="A95" r:id="rId93" xr:uid="{B60EF477-38A6-4A80-BF86-457AA885F7D9}"/>
-    <hyperlink ref="A2" r:id="rId94" xr:uid="{A57B20CD-6386-4B60-9944-587A675D840D}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{2ED6477F-0688-4D70-9365-BC7C4E376E82}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{4E965D07-00A3-4210-A3BD-0610EC11A2A9}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{AD3154FD-4E59-4F6A-AF7A-0BD20636047C}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{C83CACB8-67C6-4F79-9BDF-1044B79921D5}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{D43AE3EF-E3DA-41C8-AFC4-E5349EC8B5C5}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{4BB1437E-9B8A-40C0-B9C6-4EFE0F984E0C}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{D6BE7778-74BB-4963-ABA9-ADD3BC183450}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{5B12592E-5270-4F77-A890-6AC575B216BE}"/>
+    <hyperlink ref="A11" r:id="rId9" xr:uid="{5EDFA56F-BCE8-4595-8022-78A9EC20F81C}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{8F9FB0A6-1066-4016-99F3-F077C1A61B72}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{ECCE968F-15BA-40FE-84E4-AA690F0243C3}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{A7D770FF-8719-4845-B12A-369B078A57AF}"/>
+    <hyperlink ref="A15" r:id="rId13" xr:uid="{B8E2B792-248D-4E06-A44A-37FB0751C926}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{33FE71A4-3055-4512-9648-835FF72B73A0}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{CB5A3C4C-13D9-4B24-B195-210ED4FBE9DD}"/>
+    <hyperlink ref="A18" r:id="rId16" xr:uid="{3AC92931-509C-42A2-B8B3-B8E9825C6152}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{D481EA02-ABB2-477A-B879-64A8985E8B70}"/>
+    <hyperlink ref="A20" r:id="rId18" xr:uid="{2BA13EA5-BEF4-4BD6-9DC5-1712C7F0D6AD}"/>
+    <hyperlink ref="A21" r:id="rId19" xr:uid="{A1CC8ACA-57E9-426C-AD55-3D98FB8F4A3C}"/>
+    <hyperlink ref="A22" r:id="rId20" xr:uid="{1D7C8697-430A-4635-98F7-6C07C74C047A}"/>
+    <hyperlink ref="A23" r:id="rId21" xr:uid="{15CFAEC5-E79E-4A81-BA48-14FC39B0936A}"/>
+    <hyperlink ref="A24" r:id="rId22" xr:uid="{442ADA00-59A2-4E20-A46E-763B9C9B3C61}"/>
+    <hyperlink ref="A25" r:id="rId23" xr:uid="{780A9EF4-0D73-4CA9-9D8C-044E7EA952B6}"/>
+    <hyperlink ref="A26" r:id="rId24" xr:uid="{BCE3420B-4685-430C-BF85-F07AF758B484}"/>
+    <hyperlink ref="A27" r:id="rId25" xr:uid="{57291359-7B98-4B4C-8536-8EB7441B14A0}"/>
+    <hyperlink ref="A28" r:id="rId26" xr:uid="{9D67495D-89E1-4FDD-99B2-CC69FB31AF9E}"/>
+    <hyperlink ref="A29" r:id="rId27" xr:uid="{A226A6D0-E373-442F-AB5F-E0B292A02A8A}"/>
+    <hyperlink ref="A30" r:id="rId28" xr:uid="{41817B1D-9404-48C4-B75D-F3D8B9E0AD1D}"/>
+    <hyperlink ref="A31" r:id="rId29" xr:uid="{EB71C670-C4CE-4398-BDE7-77300FD16A0D}"/>
+    <hyperlink ref="A32" r:id="rId30" xr:uid="{D4C6CE7D-0BC7-48E8-ADDB-23A197EACE2E}"/>
+    <hyperlink ref="A33" r:id="rId31" xr:uid="{44B8E59E-0510-4D97-870C-C3C231B24295}"/>
+    <hyperlink ref="A34" r:id="rId32" xr:uid="{506D721A-9121-4CE4-BDE2-6298F5AC0A80}"/>
+    <hyperlink ref="A35" r:id="rId33" xr:uid="{3705B74A-ADF1-4299-9614-AA3121DAA70E}"/>
+    <hyperlink ref="A36" r:id="rId34" xr:uid="{BEAD36FD-1FCD-4EB6-B097-565D30DEEE06}"/>
+    <hyperlink ref="A37" r:id="rId35" xr:uid="{426CE7E4-A72D-4063-BD29-E92B5F2639B4}"/>
+    <hyperlink ref="A38" r:id="rId36" xr:uid="{D42F1856-FFB3-4C86-AB39-3C7E6526AAD3}"/>
+    <hyperlink ref="A39" r:id="rId37" xr:uid="{74522C41-48D1-4AF6-A507-54A73C6E8B60}"/>
+    <hyperlink ref="A40" r:id="rId38" xr:uid="{FD599B93-4AD7-40AE-8E60-8B8214FB0CA9}"/>
+    <hyperlink ref="A41" r:id="rId39" xr:uid="{BC65FEAA-46EB-44A4-941A-1A1ACE394565}"/>
+    <hyperlink ref="A42" r:id="rId40" xr:uid="{BDE6EB0D-79F9-44D0-8443-3D7CB8C14462}"/>
+    <hyperlink ref="A43" r:id="rId41" xr:uid="{CAC9B4DB-E9A6-4438-B269-D09E1BC8548F}"/>
+    <hyperlink ref="A44" r:id="rId42" xr:uid="{DDFA5ABF-AE8F-49FA-A3B7-21A4DE9ED7F4}"/>
+    <hyperlink ref="A45" r:id="rId43" xr:uid="{BBBA4BAB-6646-4FEC-9A4F-4C76BDB17FC1}"/>
+    <hyperlink ref="A46" r:id="rId44" xr:uid="{451C84BC-237E-4282-87A3-46FBC0F6D86D}"/>
+    <hyperlink ref="A47" r:id="rId45" xr:uid="{2F75B136-F1C2-4C12-B624-31ECE87D8A47}"/>
+    <hyperlink ref="A48" r:id="rId46" xr:uid="{CDA32D37-0E6E-4DB6-8996-1391D6B823AF}"/>
+    <hyperlink ref="A49" r:id="rId47" xr:uid="{A8E3D0EC-CE2B-49A6-825B-9F3A98A84902}"/>
+    <hyperlink ref="A50" r:id="rId48" xr:uid="{91BE7A6B-AB8E-4217-9051-99D643CFB8B9}"/>
+    <hyperlink ref="A51" r:id="rId49" xr:uid="{66C6D3CB-1799-4DC3-BA4B-9F2067186376}"/>
+    <hyperlink ref="A52" r:id="rId50" xr:uid="{967DFBB0-D1D8-4869-8CAD-65D686C4C122}"/>
+    <hyperlink ref="A53" r:id="rId51" xr:uid="{BE4394CD-4739-4374-8B48-AE4A22F6EBA8}"/>
+    <hyperlink ref="A54" r:id="rId52" xr:uid="{70FD45C9-805A-4576-B677-EFC5E8BCBEB0}"/>
+    <hyperlink ref="A55" r:id="rId53" xr:uid="{E0A82E61-FA34-4A2F-88C1-1D90A6B43CA9}"/>
+    <hyperlink ref="A56" r:id="rId54" xr:uid="{16E2E0B9-865F-47A9-A2DF-60DC29575AA3}"/>
+    <hyperlink ref="A57" r:id="rId55" xr:uid="{27711C84-8F4E-4452-8FCF-A565AFA74D4B}"/>
+    <hyperlink ref="A58" r:id="rId56" xr:uid="{062B4421-F4D8-4DD2-90E7-81C270D8DB40}"/>
+    <hyperlink ref="A59" r:id="rId57" xr:uid="{5515994B-B7C3-45F0-ACAA-B4F27271573A}"/>
+    <hyperlink ref="A60" r:id="rId58" xr:uid="{36EEE2B9-2129-4E3E-86EB-D45FF5CD0362}"/>
+    <hyperlink ref="A61" r:id="rId59" xr:uid="{8DC9732E-558E-4A1A-B05E-23B317DB8187}"/>
+    <hyperlink ref="A62" r:id="rId60" xr:uid="{DE39333C-BED3-46A7-A6C3-E74790E4838A}"/>
+    <hyperlink ref="A63" r:id="rId61" xr:uid="{EF628698-ACEB-4818-8438-8AE9DBE4E126}"/>
+    <hyperlink ref="A64" r:id="rId62" xr:uid="{A5E3A352-1658-4385-AA61-C5534A3A9587}"/>
+    <hyperlink ref="A65" r:id="rId63" xr:uid="{4AE2E7BA-0779-480A-9E10-833E8BEE6176}"/>
+    <hyperlink ref="A66" r:id="rId64" xr:uid="{B3B16C79-E44A-4AE2-B5C9-1EFD3F70716F}"/>
+    <hyperlink ref="A67" r:id="rId65" xr:uid="{03DA74CC-C5B3-4A14-A92E-53593A6ED634}"/>
+    <hyperlink ref="A68" r:id="rId66" xr:uid="{292707FA-9363-4D5D-85B0-DE717207FB57}"/>
+    <hyperlink ref="A69" r:id="rId67" xr:uid="{762A6932-B76D-4288-AAA5-AD7B947816CD}"/>
+    <hyperlink ref="A70" r:id="rId68" xr:uid="{A7A1FE0D-E7F4-4EAE-9CF9-CAFF7CD89E4B}"/>
+    <hyperlink ref="A71" r:id="rId69" xr:uid="{390820E8-74CF-4356-A8B3-BCE3EF7CD95D}"/>
+    <hyperlink ref="A72" r:id="rId70" xr:uid="{8327DA18-AD6F-40E6-ACEE-D696E19D77BE}"/>
+    <hyperlink ref="A73" r:id="rId71" xr:uid="{FB7730C5-19E4-46CB-B430-BA67FB7A8BF6}"/>
+    <hyperlink ref="A74" r:id="rId72" xr:uid="{5C886BAE-5C7E-43DC-9F0F-6D2E48017393}"/>
+    <hyperlink ref="A75" r:id="rId73" xr:uid="{DD617D6F-76F1-4B6B-A91A-BD297C6E5B2F}"/>
+    <hyperlink ref="A76" r:id="rId74" xr:uid="{149414E2-2F48-42D0-A11E-07B59A54E26C}"/>
+    <hyperlink ref="A77" r:id="rId75" xr:uid="{93D0BD43-2609-492E-AD0E-DE9EAC41013B}"/>
+    <hyperlink ref="A78" r:id="rId76" xr:uid="{6AAE379F-5B4B-4BAC-A622-2C0B9A6D27C8}"/>
+    <hyperlink ref="A79" r:id="rId77" xr:uid="{8E61AF1B-D8B7-4E8E-A65E-A37974FCCEDE}"/>
+    <hyperlink ref="A80" r:id="rId78" xr:uid="{0D32D76B-A1CC-4E22-BFB0-1657FDF52326}"/>
+    <hyperlink ref="A81" r:id="rId79" xr:uid="{88E2535D-E2EA-4BB4-B2A8-61F8D7CC7094}"/>
+    <hyperlink ref="A82" r:id="rId80" xr:uid="{B60EF477-38A6-4A80-BF86-457AA885F7D9}"/>
+    <hyperlink ref="A2" r:id="rId81" xr:uid="{A57B20CD-6386-4B60-9944-587A675D840D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId95"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId82"/>
 </worksheet>
 </file>
</xml_diff>